<commit_message>
Updated type map for loose map between SqlDbType and DbTypes. Updated excel file and made missing mappings not error out anymore.
</commit_message>
<xml_diff>
--- a/SimpleClassCreator.Tests/TypeMap.xlsx
+++ b/SimpleClassCreator.Tests/TypeMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\GitHub\simple-class-creator\SimpleClassCreator.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331CBAD1-D818-4DB3-AC48-A694EA306F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4375F1C-487C-450F-AA96-D693A83BC62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FEF33DAB-1096-477D-B7E2-06814114E96F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
   <si>
     <t>SqlDbType</t>
   </si>
@@ -234,6 +234,112 @@
   </si>
   <si>
     <t>Map</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>64-bit signed integer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fixed-length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> stream of binary data ranging between 1 and 8,000 bytes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Variable-length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> stream of binary data ranging between 1 and 8,000 bytes.</t>
+    </r>
+  </si>
+  <si>
+    <t>An unsigned numeric value that can be 0, 1, or null.</t>
+  </si>
+  <si>
+    <t>A fixed-length stream of non-Unicode characters ranging between 1 and 8,000 characters.</t>
+  </si>
+  <si>
+    <t>Date data ranging in value from January 1,1 AD through December 31, 9999 AD.</t>
+  </si>
+  <si>
+    <t>Date and time data ranging in value from January 1, 1753 to December 31, 9999 to an accuracy of 3.33 milliseconds.</t>
+  </si>
+  <si>
+    <t>Date and time data. Date value range is from January 1,1 AD through December 31, 9999 AD. Time value range is 00:00:00 through 23:59:59.9999999 with an accuracy of 100 nanoseconds.</t>
+  </si>
+  <si>
+    <t>Date and time data with time zone awareness. Date value range is from January 1,1 AD through December 31, 9999 AD. Time value range is 00:00:00 through 23:59:59.9999999 with an accuracy of 100 nanoseconds. Time zone value range is -14:00 through +14:00.</t>
+  </si>
+  <si>
+    <t>Fixed precision and scale numeric value between -10 38 -1 and 10 38 -1.</t>
+  </si>
+  <si>
+    <t>Floating point number within the range of -1.79E +308 through 1.79E +308.</t>
+  </si>
+  <si>
+    <t>32-bit signed integer.</t>
+  </si>
+  <si>
+    <t>Fixed-length stream of Unicode characters ranging between 1 and 4,000 characters.</t>
+  </si>
+  <si>
+    <t>Currency value ranging from -2 63 (or -9,223,372,036,854,775,808) to 2 63 -1 (or +9,223,372,036,854,775,807) with an accuracy to a ten-thousandth of a currency unit.</t>
+  </si>
+  <si>
+    <t>Variable-length stream of Unicode characters ranging between 1 and 4,000 characters.</t>
+  </si>
+  <si>
+    <t>Floating point number within the range of -3.40E +38 through 3.40E +38.</t>
+  </si>
+  <si>
+    <t>16-bit signed integer.</t>
+  </si>
+  <si>
+    <t>Time data based on a 24-hour clock. Time value range is 00:00:00 through 23:59:59.9999999 with an accuracy of 100 nanoseconds.</t>
+  </si>
+  <si>
+    <t>Variable-length stream of non-Unicode characters ranging between 1 and 8,000 characters.</t>
+  </si>
+  <si>
+    <t>XML value</t>
+  </si>
+  <si>
+    <t>8-bit unsigned integer</t>
   </si>
 </sst>
 </file>
@@ -650,7 +756,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A32"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +1059,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A28"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EE60C0-756B-47C6-833D-37217800E320}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,9 +1341,11 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1253,8 +1361,11 @@
       <c r="E1" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1271,26 +1382,22 @@
         <f>IF(D2&lt;&gt;"", _xlfn.CONCAT("{ SqlDbType.", B2, ", DbType.", D2, " },"), "")</f>
         <v>{ SqlDbType.BigInt, DbType.Int64 },</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E32" si="0">IF(D3&lt;&gt;"", _xlfn.CONCAT("{ SqlDbType.", B3, ", DbType.", D3, " },"), "")</f>
-        <v>{ SqlDbType.Binary, DbType.Binary },</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1304,11 +1411,14 @@
         <v>46</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E3:E32" si="0">IF(D4&lt;&gt;"", _xlfn.CONCAT("{ SqlDbType.", B4, ", DbType.", D4, " },"), "")</f>
         <v>{ SqlDbType.Bit, DbType.Boolean },</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1325,8 +1435,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Char, DbType.AnsiStringFixedLength },</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1343,8 +1456,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Date, DbType.Date },</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1361,8 +1477,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.DateTime, DbType.DateTime },</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1379,8 +1498,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.DateTime2, DbType.DateTime2 },</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1397,8 +1519,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.DateTimeOffset, DbType.DateTimeOffset },</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1415,8 +1540,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Decimal, DbType.Decimal },</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1433,8 +1561,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Float, DbType.Double },</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1446,7 +1577,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1463,8 +1594,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Int, DbType.Int32 },</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1481,8 +1615,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Money, DbType.Currency },</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1499,8 +1636,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.NChar, DbType.StringFixedLength },</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1512,7 +1652,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1529,8 +1669,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.NVarChar, DbType.String },</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1547,8 +1690,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Real, DbType.Single },</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1560,7 +1706,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1577,8 +1723,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.SmallInt, DbType.Int16 },</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1590,7 +1739,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1602,7 +1751,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1614,7 +1763,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1631,8 +1780,11 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Time, DbType.Time },</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1644,19 +1796,28 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{ SqlDbType.TinyInt, DbType.Byte },</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1668,7 +1829,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1686,19 +1847,28 @@
         <v>{ SqlDbType.UniqueIdentifier, DbType.Guid },</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>{ SqlDbType.VarBinary, DbType.Binary },</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1715,20 +1885,19 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.VarChar, DbType.AnsiString },</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1745,10 +1914,8 @@
         <f t="shared" si="0"/>
         <v>{ SqlDbType.Xml, DbType.Xml },</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>47</v>
+      <c r="F32" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
@@ -1786,5 +1953,6 @@
     <sortCondition ref="C2:C34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>